<commit_message>
Reporting Best Practices PDF download in files
follow up from Taking Google Analytics Further session
</commit_message>
<xml_diff>
--- a/files/Scout-Google-Analytics-Report-Template-2017-v2.xlsx
+++ b/files/Scout-Google-Analytics-Report-Template-2017-v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29140" yWindow="0" windowWidth="37360" windowHeight="21140" tabRatio="659"/>
+    <workbookView xWindow="28880" yWindow="3600" windowWidth="23940" windowHeight="19380" tabRatio="659" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="10" r:id="rId1"/>
@@ -1258,14 +1258,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="638">
@@ -2568,13 +2568,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>892.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>262.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2710,22 +2710,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>682.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>241.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -2864,16 +2864,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>121.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
@@ -2959,6 +2959,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3115,6 +3116,9 @@
                 <c:pt idx="14" formatCode="#,##0">
                   <c:v>1166.0</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>992.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3268,6 +3272,9 @@
                 <c:pt idx="14">
                   <c:v>992.0</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>886.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3283,11 +3290,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2075861544"/>
-        <c:axId val="-2075858568"/>
+        <c:axId val="-2142169656"/>
+        <c:axId val="-2143239560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2075861544"/>
+        <c:axId val="-2142169656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,7 +3303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2075858568"/>
+        <c:crossAx val="-2143239560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3304,7 +3311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2075858568"/>
+        <c:axId val="-2143239560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3315,13 +3322,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2075861544"/>
+        <c:crossAx val="-2142169656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3723,7 +3731,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3736,7 +3744,7 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3747,12 +3755,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" ht="14" customHeight="1">
       <c r="A2" s="26"/>
@@ -3769,10 +3777,10 @@
         <v>55</v>
       </c>
       <c r="B3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>9</v>
       </c>
       <c r="D3" s="20"/>
       <c r="F3" s="23" t="s">
@@ -3804,15 +3812,15 @@
       </c>
       <c r="B6" s="17">
         <f>VLOOKUP(B3,Overview!A:H,2,FALSE)</f>
-        <v>1166</v>
+        <v>992</v>
       </c>
       <c r="C6" s="17">
         <f>VLOOKUP(C3,Overview!A:H,2,FALSE)</f>
-        <v>901</v>
+        <v>1166</v>
       </c>
       <c r="D6" s="18">
         <f>(B6-C6)/C6</f>
-        <v>0.29411764705882354</v>
+        <v>-0.14922813036020582</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
@@ -3821,15 +3829,15 @@
       </c>
       <c r="B7" s="17">
         <f>VLOOKUP(B3,Overview!A:H,3,FALSE)</f>
-        <v>992</v>
+        <v>886</v>
       </c>
       <c r="C7" s="17">
         <f>VLOOKUP(C3,Overview!A:H,3,FALSE)</f>
-        <v>784</v>
+        <v>992</v>
       </c>
       <c r="D7" s="18">
         <f>(B7-C7)/C7</f>
-        <v>0.26530612244897961</v>
+        <v>-0.10685483870967742</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
@@ -3838,15 +3846,15 @@
       </c>
       <c r="B8" s="17">
         <f>VLOOKUP(B3,Overview!A:H,4,FALSE)</f>
-        <v>1774</v>
+        <v>0</v>
       </c>
       <c r="C8" s="17">
         <f>VLOOKUP(C3,Overview!A:H,4,FALSE)</f>
-        <v>1289</v>
+        <v>1774</v>
       </c>
       <c r="D8" s="18">
         <f>(B8-C8)/C8</f>
-        <v>0.37626066718386347</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
@@ -3855,32 +3863,32 @@
       </c>
       <c r="B9" s="17">
         <f>VLOOKUP(B3,Overview!A:H,5,FALSE)</f>
-        <v>1.52</v>
+        <v>0</v>
       </c>
       <c r="C9" s="17">
         <f>VLOOKUP(C3,Overview!A:H,5,FALSE)</f>
-        <v>1.43</v>
+        <v>1.52</v>
       </c>
       <c r="D9" s="18">
         <f>(B9-C9)/C9</f>
-        <v>6.2937062937062999E-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="33">
         <f>VLOOKUP(B3,Overview!A:H,6,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="33">
+        <f>VLOOKUP(C3,Overview!A:H,6,FALSE)</f>
         <v>7.7546296296296304E-4</v>
-      </c>
-      <c r="C10" s="35">
-        <f>VLOOKUP(C3,Overview!A:H,6,FALSE)</f>
-        <v>7.5231481481481471E-4</v>
       </c>
       <c r="D10" s="18">
         <f>(B10-C10)/C10</f>
-        <v>3.0769230769231021E-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
@@ -3889,15 +3897,15 @@
       </c>
       <c r="B11" s="19">
         <f>VLOOKUP(B3,Overview!A:H,7,FALSE)</f>
-        <v>0.78129999999999999</v>
+        <v>0</v>
       </c>
       <c r="C11" s="19">
         <f>VLOOKUP(C3,Overview!A:H,7,FALSE)</f>
-        <v>0.80689999999999995</v>
-      </c>
-      <c r="D11" s="18">
+        <v>0.78129999999999999</v>
+      </c>
+      <c r="D11" s="18" t="e">
         <f t="shared" ref="D11" si="0">(C11-B11)/B11</f>
-        <v>3.2765902982209084E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
@@ -3906,15 +3914,15 @@
       </c>
       <c r="B12" s="19">
         <f>VLOOKUP(B3,Overview!A:H,8,FALSE)</f>
-        <v>0.82420000000000004</v>
+        <v>0</v>
       </c>
       <c r="C12" s="19">
         <f>VLOOKUP(C3,Overview!A:H,8,FALSE)</f>
-        <v>0.83460000000000001</v>
+        <v>0.82420000000000004</v>
       </c>
       <c r="D12" s="18">
         <f>(B12-C12)/C12</f>
-        <v>-1.2461059190031111E-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
@@ -3939,15 +3947,15 @@
       </c>
       <c r="B15" s="17">
         <f>VLOOKUP(B3,Mobile!A:D,2,FALSE)</f>
-        <v>892</v>
+        <v>0</v>
       </c>
       <c r="C15" s="17">
         <f>VLOOKUP(C3,Mobile!A:D,2,FALSE)</f>
-        <v>752</v>
+        <v>892</v>
       </c>
       <c r="D15" s="18">
         <f>(B15-C15)/C15</f>
-        <v>0.18617021276595744</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
@@ -3956,15 +3964,15 @@
       </c>
       <c r="B16" s="17">
         <f>VLOOKUP(B3,Mobile!A:D,3,FALSE)</f>
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="C16" s="17">
         <f>VLOOKUP(C3,Mobile!A:D,3,FALSE)</f>
-        <v>134</v>
+        <v>262</v>
       </c>
       <c r="D16" s="18">
         <f>(B16-C16)/C16</f>
-        <v>0.95522388059701491</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -3973,15 +3981,15 @@
       </c>
       <c r="B17" s="17">
         <f>VLOOKUP(B3,Mobile!A:D,4,FALSE)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C17" s="17">
         <f>VLOOKUP(C3,Mobile!A:D,4,FALSE)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D17" s="18">
         <f>(B17-C17)/C17</f>
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -4006,15 +4014,15 @@
       </c>
       <c r="B20" s="17">
         <f>VLOOKUP($B$3,Channels!A:L,2,FALSE)</f>
-        <v>682</v>
+        <v>0</v>
       </c>
       <c r="C20" s="17">
         <f>VLOOKUP($C$3,Channels!A:L,2,FALSE)</f>
-        <v>502</v>
+        <v>682</v>
       </c>
       <c r="D20" s="18">
         <f t="shared" ref="D20:D27" si="1">(B20-C20)/C20</f>
-        <v>0.35856573705179284</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
@@ -4040,15 +4048,15 @@
       </c>
       <c r="B22" s="17">
         <f>VLOOKUP($B$3,Channels!A:L,7,FALSE)</f>
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="C22" s="17">
         <f>VLOOKUP($C$3,Channels!A:L,7,FALSE)</f>
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="D22" s="18">
         <f t="shared" si="1"/>
-        <v>-0.11721611721611722</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -4057,15 +4065,15 @@
       </c>
       <c r="B23" s="17">
         <f>VLOOKUP($B$3,Channels!A:L,8,FALSE)</f>
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="C23" s="17">
         <f>VLOOKUP($C$3,Channels!A:L,8,FALSE)</f>
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D23" s="18">
         <f t="shared" si="1"/>
-        <v>0.28846153846153844</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -4074,15 +4082,15 @@
       </c>
       <c r="B24" s="17">
         <f>VLOOKUP($B$3,Channels!A:L,9,FALSE)</f>
-        <v>149</v>
+        <v>0</v>
       </c>
       <c r="C24" s="17">
         <f>VLOOKUP($C$3,Channels!A:L,9,FALSE)</f>
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="D24" s="18">
         <f t="shared" si="1"/>
-        <v>1.6140350877192982</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -4091,15 +4099,15 @@
       </c>
       <c r="B25" s="17">
         <f>VLOOKUP($B$3,Channels!A:L,10,FALSE)</f>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C25" s="17">
         <f>VLOOKUP($C$3,Channels!A:L,10,FALSE)</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D25" s="18">
         <f t="shared" si="1"/>
-        <v>0.58823529411764708</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -4158,15 +4166,15 @@
       </c>
       <c r="B30" s="17">
         <f>VLOOKUP($B$3,Social!A:K,2,FALSE)</f>
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="C30" s="17">
         <f>VLOOKUP($C$3,Social!A:K,2,FALSE)</f>
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="D30" s="18">
         <f t="shared" ref="D30:D39" si="2">(B30-C30)/C30</f>
-        <v>1.42</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
@@ -4175,15 +4183,15 @@
       </c>
       <c r="B31" s="17">
         <f>VLOOKUP($B$3,Social!A:K,3,FALSE)</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C31" s="17">
         <f>VLOOKUP($C$3,Social!A:K,3,FALSE)</f>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D31" s="18">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
@@ -4192,15 +4200,15 @@
       </c>
       <c r="B32" s="17">
         <f>VLOOKUP($B$3,Social!A:K,4,FALSE)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C32" s="17">
         <f>VLOOKUP($C$3,Social!A:K,4,FALSE)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D32" s="18">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
@@ -4209,15 +4217,15 @@
       </c>
       <c r="B33" s="17">
         <f>VLOOKUP($B$3,Social!A:K,5,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="17">
         <f>VLOOKUP($C$3,Social!A:K,5,FALSE)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D33" s="18">
         <f t="shared" si="2"/>
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
@@ -4577,8 +4585,8 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4588,16 +4596,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="29" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -4851,8 +4859,12 @@
       <c r="A18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="3">
+        <v>992</v>
+      </c>
+      <c r="C18" s="3">
+        <v>886</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
       <c r="F18" s="28"/>
@@ -5132,32 +5144,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="29" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -5735,7 +5747,7 @@
   </sheetPr>
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D38"/>
     </sheetView>
   </sheetViews>
@@ -5745,12 +5757,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" ht="29" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -6105,20 +6117,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="29" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -6817,19 +6829,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="29" customHeight="1">
       <c r="A2" s="2" t="s">

</xml_diff>